<commit_message>
Added select sheet function.
</commit_message>
<xml_diff>
--- a/XLSX/test.xlsx
+++ b/XLSX/test.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/da9bcc817bfc68d1/Dokumente/Code/Code - Diverse Module/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Excel2json\excel2json\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B79C8635-9334-4B04-AEE7-4ACAC5FD88F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682CBAD8-8FDA-49EE-8D86-42FD9A8079E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="18820" xr2:uid="{DF3D8B01-41F0-4470-B847-09D720B0B94E}"/>
+    <workbookView xWindow="40125" yWindow="3570" windowWidth="21600" windowHeight="13665" activeTab="1" xr2:uid="{DF3D8B01-41F0-4470-B847-09D720B0B94E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
   <si>
     <t>Spalte1</t>
   </si>
@@ -216,6 +217,9 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -569,13 +573,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{447D9872-28BF-4563-97E2-2B9AD3692DB5}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -604,7 +608,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -633,7 +637,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -662,7 +666,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -685,7 +689,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -708,7 +712,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -731,7 +735,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -754,7 +758,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -777,7 +781,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -798,6 +802,38 @@
       </c>
       <c r="G9" t="s">
         <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF5FDC9-3B42-48E8-A384-1876AC27FEC1}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>